<commit_message>
Added Lousiana line list and estimate of theta-boosting parameter
https://wiki.idmod.org/pages/viewpage.action?pageId=77037995
</commit_message>
<xml_diff>
--- a/data/Louisiana1957/householdSeroconversion.xlsx
+++ b/data/Louisiana1957/householdSeroconversion.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfamulare\Dropbox (IDM)\VaccineNetworkTransmissionPaper\data\Louisiana1957\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfamulare\github\cessationStability\data\Louisiana1957\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11976" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="seroconversion" sheetId="1" r:id="rId1"/>
-    <sheet name="preExposureAntibodyTiter" sheetId="2" r:id="rId2"/>
-    <sheet name="postExposureAntibodyTiter" sheetId="3" r:id="rId3"/>
+    <sheet name="preExposureAntibodyTiterPDF" sheetId="2" r:id="rId2"/>
+    <sheet name="postExposureAntibodyTiterPDF" sheetId="3" r:id="rId3"/>
+    <sheet name="prePostAntibodyLineList" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>category</t>
   </si>
@@ -71,6 +72,12 @@
   </si>
   <si>
     <t>* can't disambiguate by age</t>
+  </si>
+  <si>
+    <t>preExposureTiter</t>
+  </si>
+  <si>
+    <t>postExposureTiter</t>
   </si>
 </sst>
 </file>
@@ -424,16 +431,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -467,7 +474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -481,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -495,7 +502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -512,7 +519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -542,9 +549,9 @@
       <selection activeCell="E2" sqref="E2:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -555,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -566,7 +573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -574,7 +581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
@@ -582,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -590,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
@@ -598,7 +605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>40</v>
       </c>
@@ -606,7 +613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
@@ -614,7 +621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>160</v>
       </c>
@@ -622,7 +629,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>320</v>
       </c>
@@ -630,7 +637,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>640</v>
       </c>
@@ -638,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1280</v>
       </c>
@@ -646,7 +653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2560</v>
       </c>
@@ -654,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5210</v>
       </c>
@@ -672,12 +679,12 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -688,7 +695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -699,7 +706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -707,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -715,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20</v>
       </c>
@@ -723,7 +730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40</v>
       </c>
@@ -731,7 +738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>80</v>
       </c>
@@ -739,7 +746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>160</v>
       </c>
@@ -747,7 +754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>320</v>
       </c>
@@ -755,7 +762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>640</v>
       </c>
@@ -763,7 +770,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1280</v>
       </c>
@@ -771,7 +778,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2560</v>
       </c>
@@ -779,7 +786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5210</v>
       </c>
@@ -787,7 +794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10240</v>
       </c>
@@ -795,7 +802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20480</v>
       </c>
@@ -803,12 +810,2252 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>40960</v>
       </c>
       <c r="B16">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C277"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>20</v>
+      </c>
+      <c r="B48">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>20</v>
+      </c>
+      <c r="B51">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>20</v>
+      </c>
+      <c r="B52">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>20</v>
+      </c>
+      <c r="B53">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>20</v>
+      </c>
+      <c r="B54">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>20</v>
+      </c>
+      <c r="B56">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>20</v>
+      </c>
+      <c r="B57">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>40</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>40</v>
+      </c>
+      <c r="B59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>40</v>
+      </c>
+      <c r="B60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>40</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>40</v>
+      </c>
+      <c r="B62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>40</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>40</v>
+      </c>
+      <c r="B64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>40</v>
+      </c>
+      <c r="B65">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>40</v>
+      </c>
+      <c r="B66">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>40</v>
+      </c>
+      <c r="B67">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>40</v>
+      </c>
+      <c r="B68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>40</v>
+      </c>
+      <c r="B69">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>40</v>
+      </c>
+      <c r="B70">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>40</v>
+      </c>
+      <c r="B71">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>40</v>
+      </c>
+      <c r="B72">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>40</v>
+      </c>
+      <c r="B73">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>40</v>
+      </c>
+      <c r="B74">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>40</v>
+      </c>
+      <c r="B75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>40</v>
+      </c>
+      <c r="B76">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>40</v>
+      </c>
+      <c r="B77">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>40</v>
+      </c>
+      <c r="B78">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>40</v>
+      </c>
+      <c r="B79">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>40</v>
+      </c>
+      <c r="B80">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>40</v>
+      </c>
+      <c r="B81">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>40</v>
+      </c>
+      <c r="B82">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>40</v>
+      </c>
+      <c r="B83">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>40</v>
+      </c>
+      <c r="B84">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>40</v>
+      </c>
+      <c r="B85">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>40</v>
+      </c>
+      <c r="B86">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>80</v>
+      </c>
+      <c r="B88">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>80</v>
+      </c>
+      <c r="B89">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>80</v>
+      </c>
+      <c r="B90">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>80</v>
+      </c>
+      <c r="B91">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>80</v>
+      </c>
+      <c r="B92">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>80</v>
+      </c>
+      <c r="B93">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>80</v>
+      </c>
+      <c r="B94">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>80</v>
+      </c>
+      <c r="B95">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>80</v>
+      </c>
+      <c r="B96">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>80</v>
+      </c>
+      <c r="B97">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>80</v>
+      </c>
+      <c r="B98">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>80</v>
+      </c>
+      <c r="B99">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>80</v>
+      </c>
+      <c r="B100">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>80</v>
+      </c>
+      <c r="B101">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>80</v>
+      </c>
+      <c r="B102">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>80</v>
+      </c>
+      <c r="B103">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>80</v>
+      </c>
+      <c r="B104">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>80</v>
+      </c>
+      <c r="B105">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>80</v>
+      </c>
+      <c r="B106">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>80</v>
+      </c>
+      <c r="B107">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>80</v>
+      </c>
+      <c r="B108">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>80</v>
+      </c>
+      <c r="B109">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>80</v>
+      </c>
+      <c r="B110">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>80</v>
+      </c>
+      <c r="B111">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>80</v>
+      </c>
+      <c r="B112">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>80</v>
+      </c>
+      <c r="B113">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>80</v>
+      </c>
+      <c r="B114">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>80</v>
+      </c>
+      <c r="B115">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>80</v>
+      </c>
+      <c r="B116">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>80</v>
+      </c>
+      <c r="B117">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>80</v>
+      </c>
+      <c r="B118">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>80</v>
+      </c>
+      <c r="B119">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>80</v>
+      </c>
+      <c r="B120">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>80</v>
+      </c>
+      <c r="B121">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>80</v>
+      </c>
+      <c r="B122">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>80</v>
+      </c>
+      <c r="B123">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>80</v>
+      </c>
+      <c r="B124">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>80</v>
+      </c>
+      <c r="B125">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>80</v>
+      </c>
+      <c r="B126">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>80</v>
+      </c>
+      <c r="B127">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>80</v>
+      </c>
+      <c r="B128">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>80</v>
+      </c>
+      <c r="B129">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>80</v>
+      </c>
+      <c r="B130">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>80</v>
+      </c>
+      <c r="B131">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>80</v>
+      </c>
+      <c r="B132">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>80</v>
+      </c>
+      <c r="B133">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>160</v>
+      </c>
+      <c r="B134">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>160</v>
+      </c>
+      <c r="B135">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>160</v>
+      </c>
+      <c r="B136">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>160</v>
+      </c>
+      <c r="B137">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>160</v>
+      </c>
+      <c r="B138">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>160</v>
+      </c>
+      <c r="B139">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>160</v>
+      </c>
+      <c r="B140">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>160</v>
+      </c>
+      <c r="B141">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>160</v>
+      </c>
+      <c r="B142">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>160</v>
+      </c>
+      <c r="B143">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>160</v>
+      </c>
+      <c r="B144">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>160</v>
+      </c>
+      <c r="B145">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>160</v>
+      </c>
+      <c r="B146">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>160</v>
+      </c>
+      <c r="B147">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>160</v>
+      </c>
+      <c r="B148">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>160</v>
+      </c>
+      <c r="B149">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>160</v>
+      </c>
+      <c r="B150">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>160</v>
+      </c>
+      <c r="B151">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>160</v>
+      </c>
+      <c r="B152">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>160</v>
+      </c>
+      <c r="B153">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>160</v>
+      </c>
+      <c r="B154">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>160</v>
+      </c>
+      <c r="B155">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>160</v>
+      </c>
+      <c r="B156">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>160</v>
+      </c>
+      <c r="B157">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>160</v>
+      </c>
+      <c r="B158">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>160</v>
+      </c>
+      <c r="B159">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>160</v>
+      </c>
+      <c r="B160">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>160</v>
+      </c>
+      <c r="B163">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>160</v>
+      </c>
+      <c r="B164">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>160</v>
+      </c>
+      <c r="B165">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>320</v>
+      </c>
+      <c r="B166">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>320</v>
+      </c>
+      <c r="B167">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>320</v>
+      </c>
+      <c r="B168">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>320</v>
+      </c>
+      <c r="B169">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>320</v>
+      </c>
+      <c r="B170">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>320</v>
+      </c>
+      <c r="B171">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>320</v>
+      </c>
+      <c r="B172">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>320</v>
+      </c>
+      <c r="B173">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>320</v>
+      </c>
+      <c r="B174">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>320</v>
+      </c>
+      <c r="B175">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>320</v>
+      </c>
+      <c r="B176">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>320</v>
+      </c>
+      <c r="B177">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>320</v>
+      </c>
+      <c r="B178">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>320</v>
+      </c>
+      <c r="B179">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>320</v>
+      </c>
+      <c r="B180">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>320</v>
+      </c>
+      <c r="B181">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>320</v>
+      </c>
+      <c r="B182">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>320</v>
+      </c>
+      <c r="B183">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>320</v>
+      </c>
+      <c r="B184">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>320</v>
+      </c>
+      <c r="B185">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>320</v>
+      </c>
+      <c r="B186">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>320</v>
+      </c>
+      <c r="B187">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>320</v>
+      </c>
+      <c r="B188">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>320</v>
+      </c>
+      <c r="B189">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>320</v>
+      </c>
+      <c r="B190">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>320</v>
+      </c>
+      <c r="B191">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>320</v>
+      </c>
+      <c r="B192">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>320</v>
+      </c>
+      <c r="B193">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>320</v>
+      </c>
+      <c r="B194">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>320</v>
+      </c>
+      <c r="B195">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>320</v>
+      </c>
+      <c r="B196">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>320</v>
+      </c>
+      <c r="B197">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>320</v>
+      </c>
+      <c r="B198">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>320</v>
+      </c>
+      <c r="B199">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>320</v>
+      </c>
+      <c r="B200">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>320</v>
+      </c>
+      <c r="B201">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>320</v>
+      </c>
+      <c r="B202">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>320</v>
+      </c>
+      <c r="B203">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>320</v>
+      </c>
+      <c r="B204">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>320</v>
+      </c>
+      <c r="B205">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>320</v>
+      </c>
+      <c r="B206">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>320</v>
+      </c>
+      <c r="B207">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>320</v>
+      </c>
+      <c r="B208">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>320</v>
+      </c>
+      <c r="B209">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>320</v>
+      </c>
+      <c r="B210">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>320</v>
+      </c>
+      <c r="B211">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>320</v>
+      </c>
+      <c r="B212">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>320</v>
+      </c>
+      <c r="B213">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>320</v>
+      </c>
+      <c r="B214">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>320</v>
+      </c>
+      <c r="B215">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>320</v>
+      </c>
+      <c r="B216">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>320</v>
+      </c>
+      <c r="B217">
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>320</v>
+      </c>
+      <c r="B218">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>640</v>
+      </c>
+      <c r="B219">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>640</v>
+      </c>
+      <c r="B220">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>640</v>
+      </c>
+      <c r="B221">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>640</v>
+      </c>
+      <c r="B222">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>640</v>
+      </c>
+      <c r="B223">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>640</v>
+      </c>
+      <c r="B224">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>640</v>
+      </c>
+      <c r="B225">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>640</v>
+      </c>
+      <c r="B226">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>640</v>
+      </c>
+      <c r="B227">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>640</v>
+      </c>
+      <c r="B228">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>640</v>
+      </c>
+      <c r="B229">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>640</v>
+      </c>
+      <c r="B230">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>640</v>
+      </c>
+      <c r="B231">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>640</v>
+      </c>
+      <c r="B232">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>640</v>
+      </c>
+      <c r="B233">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>640</v>
+      </c>
+      <c r="B234">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>640</v>
+      </c>
+      <c r="B235">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>640</v>
+      </c>
+      <c r="B236">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>1280</v>
+      </c>
+      <c r="B237">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>1280</v>
+      </c>
+      <c r="B238">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>1280</v>
+      </c>
+      <c r="B239">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>1280</v>
+      </c>
+      <c r="B240">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>1280</v>
+      </c>
+      <c r="B241">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>1280</v>
+      </c>
+      <c r="B242">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>1280</v>
+      </c>
+      <c r="B243">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>1280</v>
+      </c>
+      <c r="B244">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>1280</v>
+      </c>
+      <c r="B245">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>1280</v>
+      </c>
+      <c r="B246">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>1280</v>
+      </c>
+      <c r="B247">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>1280</v>
+      </c>
+      <c r="B248">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>1280</v>
+      </c>
+      <c r="B249">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>1280</v>
+      </c>
+      <c r="B250">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>1280</v>
+      </c>
+      <c r="B251">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>1280</v>
+      </c>
+      <c r="B252">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>1280</v>
+      </c>
+      <c r="B253">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>1280</v>
+      </c>
+      <c r="B254">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>1280</v>
+      </c>
+      <c r="B255">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>1280</v>
+      </c>
+      <c r="B256">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>1280</v>
+      </c>
+      <c r="B257">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>1280</v>
+      </c>
+      <c r="B258">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>2560</v>
+      </c>
+      <c r="B259">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>2560</v>
+      </c>
+      <c r="B260">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>2560</v>
+      </c>
+      <c r="B261">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>2560</v>
+      </c>
+      <c r="B262">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>2560</v>
+      </c>
+      <c r="B263">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>2560</v>
+      </c>
+      <c r="B264">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>2560</v>
+      </c>
+      <c r="B265">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>2560</v>
+      </c>
+      <c r="B266">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>2560</v>
+      </c>
+      <c r="B267">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>2560</v>
+      </c>
+      <c r="B268">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>2560</v>
+      </c>
+      <c r="B269">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>5120</v>
+      </c>
+      <c r="B270">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>5120</v>
+      </c>
+      <c r="B271">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>5120</v>
+      </c>
+      <c r="B272">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>5120</v>
+      </c>
+      <c r="B273">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>5120</v>
+      </c>
+      <c r="B274">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>5120</v>
+      </c>
+      <c r="B275">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>5120</v>
+      </c>
+      <c r="B276">
+        <v>5120</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>5120</v>
+      </c>
+      <c r="B277">
+        <v>10240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>